<commit_message>
Applied the fix to the proper excel file this time.
</commit_message>
<xml_diff>
--- a/CivilWarNarrative/bin/SoldierStory.xlsx
+++ b/CivilWarNarrative/bin/SoldierStory.xlsx
@@ -1136,7 +1136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="410">
   <si>
     <t>titleslide</t>
   </si>
@@ -1526,9 +1526,6 @@
   </si>
   <si>
     <t>buy-vest</t>
-  </si>
-  <si>
-    <t>buy-filter</t>
   </si>
   <si>
     <t>poker-playing</t>
@@ -2573,6 +2570,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2620,9 +2620,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3178,8 +3175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AT106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3230,16 +3227,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" ht="72" customHeight="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="24"/>
       <c r="C1" s="39" t="s">
         <v>116</v>
       </c>
       <c r="D1" s="39"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:46" ht="15.75" customHeight="1">
       <c r="A2" t="s">
@@ -3252,48 +3249,48 @@
       <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:46" ht="15" customHeight="1">
-      <c r="H3" s="29" t="s">
+      <c r="H3" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="32" t="s">
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="U3" s="34"/>
-      <c r="V3" s="35" t="s">
+      <c r="P3" s="34"/>
+      <c r="Q3" s="34"/>
+      <c r="R3" s="34"/>
+      <c r="S3" s="34"/>
+      <c r="T3" s="34"/>
+      <c r="U3" s="35"/>
+      <c r="V3" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="W3" s="36"/>
-      <c r="X3" s="36"/>
-      <c r="Y3" s="36"/>
-      <c r="Z3" s="36"/>
-      <c r="AA3" s="36"/>
-      <c r="AB3" s="37"/>
-      <c r="AC3" s="26" t="s">
+      <c r="W3" s="37"/>
+      <c r="X3" s="37"/>
+      <c r="Y3" s="37"/>
+      <c r="Z3" s="37"/>
+      <c r="AA3" s="37"/>
+      <c r="AB3" s="38"/>
+      <c r="AC3" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="AD3" s="27"/>
-      <c r="AE3" s="27"/>
-      <c r="AF3" s="27"/>
-      <c r="AG3" s="27"/>
-      <c r="AH3" s="27"/>
-      <c r="AI3" s="28"/>
-      <c r="AJ3" s="24" t="s">
+      <c r="AD3" s="28"/>
+      <c r="AE3" s="28"/>
+      <c r="AF3" s="28"/>
+      <c r="AG3" s="28"/>
+      <c r="AH3" s="28"/>
+      <c r="AI3" s="29"/>
+      <c r="AJ3" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="AK3" s="25"/>
-      <c r="AL3" s="25"/>
-      <c r="AM3" s="25"/>
+      <c r="AK3" s="26"/>
+      <c r="AL3" s="26"/>
+      <c r="AM3" s="26"/>
     </row>
     <row r="4" spans="1:46">
       <c r="A4" t="s">
@@ -3422,14 +3419,14 @@
         <v>1</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>2</v>
@@ -3486,14 +3483,14 @@
         <v>41</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>2</v>
@@ -3554,10 +3551,10 @@
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>2</v>
@@ -3619,16 +3616,16 @@
         <v>41</v>
       </c>
       <c r="C8" s="19" t="s">
+        <v>405</v>
+      </c>
+      <c r="D8" s="17" t="s">
         <v>406</v>
       </c>
-      <c r="D8" s="17" t="s">
-        <v>407</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>2</v>
@@ -3681,13 +3678,13 @@
         <v>115</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>2</v>
@@ -3743,10 +3740,10 @@
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>2</v>
@@ -3770,7 +3767,7 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="9"/>
       <c r="R10" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="S10" s="1" t="s">
         <v>58</v>
@@ -3828,10 +3825,10 @@
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>2</v>
@@ -3893,14 +3890,14 @@
         <v>41</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>2</v>
@@ -3920,7 +3917,7 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="9"/>
       <c r="R12" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="S12" s="1" t="s">
         <v>61</v>
@@ -3955,14 +3952,14 @@
         <v>41</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>2</v>
@@ -3974,7 +3971,7 @@
         <v>3</v>
       </c>
       <c r="L13" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M13" s="11"/>
       <c r="N13" s="11"/>
@@ -4006,20 +4003,20 @@
     </row>
     <row r="14" spans="1:46" s="15" customFormat="1">
       <c r="A14" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>2</v>
@@ -4028,10 +4025,10 @@
       <c r="I14" s="11"/>
       <c r="J14" s="13"/>
       <c r="K14" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L14" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="M14" s="11"/>
       <c r="N14" s="11"/>
@@ -4039,10 +4036,10 @@
       <c r="P14" s="11"/>
       <c r="Q14" s="13"/>
       <c r="R14" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="S14" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="T14" s="11"/>
       <c r="U14" s="11"/>
@@ -4067,20 +4064,20 @@
     </row>
     <row r="15" spans="1:46" s="15" customFormat="1">
       <c r="A15" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>2</v>
@@ -4092,7 +4089,7 @@
         <v>3</v>
       </c>
       <c r="L15" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M15" s="11"/>
       <c r="N15" s="11"/>
@@ -4124,22 +4121,22 @@
     </row>
     <row r="16" spans="1:46" s="15" customFormat="1" ht="45">
       <c r="A16" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G16" s="11" t="s">
         <v>2</v>
@@ -4151,7 +4148,7 @@
         <v>3</v>
       </c>
       <c r="L16" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="M16" s="11"/>
       <c r="N16" s="11"/>
@@ -4183,20 +4180,20 @@
     </row>
     <row r="17" spans="1:39" s="15" customFormat="1">
       <c r="A17" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>2</v>
@@ -4208,7 +4205,7 @@
         <v>3</v>
       </c>
       <c r="L17" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M17" s="11"/>
       <c r="N17" s="11"/>
@@ -4240,20 +4237,20 @@
     </row>
     <row r="18" spans="1:39" s="15" customFormat="1">
       <c r="A18" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>2</v>
@@ -4265,7 +4262,7 @@
         <v>3</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="M18" s="11"/>
       <c r="N18" s="11"/>
@@ -4297,20 +4294,20 @@
     </row>
     <row r="19" spans="1:39" s="15" customFormat="1">
       <c r="A19" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D19" s="17"/>
       <c r="E19" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G19" s="11" t="s">
         <v>2</v>
@@ -4322,7 +4319,7 @@
         <v>3</v>
       </c>
       <c r="L19" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="M19" s="11"/>
       <c r="N19" s="11"/>
@@ -4354,20 +4351,20 @@
     </row>
     <row r="20" spans="1:39" s="15" customFormat="1">
       <c r="A20" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>78</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G20" s="11" t="s">
         <v>2</v>
@@ -4413,14 +4410,14 @@
         <v>41</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D21" s="17"/>
       <c r="E21" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>2</v>
@@ -4440,7 +4437,7 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="9"/>
       <c r="R21" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="S21" s="1" t="s">
         <v>61</v>
@@ -4474,16 +4471,16 @@
         <v>41</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="F22" s="21" t="s">
         <v>339</v>
-      </c>
-      <c r="F22" s="21" t="s">
-        <v>340</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>2</v>
@@ -4503,7 +4500,7 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="9"/>
       <c r="R22" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="S22" s="1" t="s">
         <v>61</v>
@@ -4537,16 +4534,16 @@
         <v>41</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="F23" s="21" t="s">
         <v>300</v>
-      </c>
-      <c r="F23" s="21" t="s">
-        <v>301</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>2</v>
@@ -4566,7 +4563,7 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="9"/>
       <c r="R23" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="S23" s="1" t="s">
         <v>61</v>
@@ -4600,16 +4597,16 @@
         <v>41</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="F24" s="21" t="s">
         <v>339</v>
-      </c>
-      <c r="F24" s="21" t="s">
-        <v>340</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>2</v>
@@ -4621,7 +4618,7 @@
         <v>3</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
@@ -4653,20 +4650,20 @@
     </row>
     <row r="25" spans="1:39">
       <c r="A25" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D25" s="17"/>
       <c r="E25" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="F25" s="21" t="s">
         <v>339</v>
-      </c>
-      <c r="F25" s="21" t="s">
-        <v>340</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>2</v>
@@ -4715,14 +4712,14 @@
         <v>41</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>2</v>
@@ -4776,16 +4773,16 @@
         <v>41</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>2</v>
@@ -4794,7 +4791,7 @@
       <c r="I27" s="1"/>
       <c r="J27" s="9"/>
       <c r="K27" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>65</v>
@@ -4805,7 +4802,7 @@
       <c r="P27" s="1"/>
       <c r="Q27" s="9"/>
       <c r="R27" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="S27" s="1" t="s">
         <v>120</v>
@@ -4839,16 +4836,16 @@
         <v>41</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>88</v>
@@ -4860,7 +4857,7 @@
       </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
@@ -4871,7 +4868,7 @@
       </c>
       <c r="R28" s="1"/>
       <c r="S28" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="T28" s="1"/>
       <c r="U28" s="1"/>
@@ -4896,20 +4893,20 @@
     </row>
     <row r="29" spans="1:39">
       <c r="A29" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D29" s="17"/>
       <c r="E29" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>2</v>
@@ -4953,20 +4950,20 @@
     </row>
     <row r="30" spans="1:39">
       <c r="A30" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D30" s="17"/>
       <c r="E30" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>2</v>
@@ -5016,14 +5013,14 @@
         <v>78</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D31" s="17"/>
       <c r="E31" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>2</v>
@@ -5069,16 +5066,16 @@
         <v>41</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>86</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>2</v>
@@ -5128,16 +5125,16 @@
         <v>41</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>86</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>2</v>
@@ -5187,16 +5184,16 @@
         <v>41</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D34" s="17" t="s">
         <v>124</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>2</v>
@@ -5250,10 +5247,10 @@
       </c>
       <c r="D35" s="17"/>
       <c r="E35" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>89</v>
@@ -5313,16 +5310,16 @@
         <v>41</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>2</v>
@@ -5372,16 +5369,16 @@
         <v>41</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>2</v>
@@ -5431,14 +5428,14 @@
         <v>41</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D38" s="17"/>
       <c r="E38" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>88</v>
@@ -5461,7 +5458,7 @@
       </c>
       <c r="R38" s="1"/>
       <c r="S38" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="T38" s="1"/>
       <c r="U38" s="1"/>
@@ -5496,16 +5493,16 @@
         <v>41</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>89</v>
@@ -5563,16 +5560,16 @@
         <v>41</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>88</v>
@@ -5626,16 +5623,16 @@
         <v>41</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>88</v>
@@ -5683,20 +5680,20 @@
     </row>
     <row r="42" spans="1:39">
       <c r="A42" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D42" s="17"/>
       <c r="E42" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>2</v>
@@ -5705,46 +5702,46 @@
       <c r="I42" s="1"/>
       <c r="J42" s="9"/>
       <c r="K42" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L42" s="1" t="s">
         <v>129</v>
       </c>
       <c r="M42" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="N42" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="N42" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
       <c r="Q42" s="9"/>
       <c r="R42" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="S42" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="S42" s="1" t="s">
-        <v>219</v>
-      </c>
       <c r="T42" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="U42" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V42" s="1"/>
       <c r="W42" s="1"/>
       <c r="X42" s="9"/>
       <c r="Y42" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Z42" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AA42" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="AB42" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="AB42" s="1" t="s">
-        <v>245</v>
       </c>
       <c r="AC42" s="1"/>
       <c r="AD42" s="1"/>
@@ -5766,14 +5763,14 @@
         <v>41</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D43" s="17"/>
       <c r="E43" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>88</v>
@@ -5821,20 +5818,20 @@
     </row>
     <row r="44" spans="1:39">
       <c r="A44" s="1" t="s">
-        <v>130</v>
+        <v>218</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D44" s="17"/>
       <c r="E44" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>88</v>
@@ -5888,14 +5885,14 @@
         <v>41</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D45" s="17"/>
       <c r="E45" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>2</v>
@@ -5907,7 +5904,7 @@
         <v>96</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
@@ -5918,13 +5915,13 @@
         <v>106</v>
       </c>
       <c r="S45" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="T45" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="U45" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="U45" s="1" t="s">
-        <v>245</v>
       </c>
       <c r="V45" s="1"/>
       <c r="W45" s="1"/>
@@ -5947,20 +5944,20 @@
     </row>
     <row r="46" spans="1:39">
       <c r="A46" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D46" s="17"/>
       <c r="E46" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>88</v>
@@ -5972,7 +5969,7 @@
       </c>
       <c r="K46" s="1"/>
       <c r="L46" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M46" s="1" t="s">
         <v>98</v>
@@ -5987,7 +5984,7 @@
       </c>
       <c r="R46" s="1"/>
       <c r="S46" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="T46" s="1" t="s">
         <v>98</v>
@@ -6016,7 +6013,7 @@
     </row>
     <row r="47" spans="1:39">
       <c r="A47" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>41</v>
@@ -6026,10 +6023,10 @@
       </c>
       <c r="D47" s="17"/>
       <c r="E47" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>88</v>
@@ -6077,20 +6074,20 @@
     </row>
     <row r="48" spans="1:39" ht="45">
       <c r="A48" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D48" s="17"/>
       <c r="E48" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>88</v>
@@ -6138,20 +6135,20 @@
     </row>
     <row r="49" spans="1:39" s="15" customFormat="1" ht="30">
       <c r="A49" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B49" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D49" s="17"/>
       <c r="E49" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G49" s="11" t="s">
         <v>89</v>
@@ -6165,7 +6162,7 @@
       <c r="J49" s="13"/>
       <c r="K49" s="11"/>
       <c r="L49" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M49" s="11"/>
       <c r="N49" s="11"/>
@@ -6178,7 +6175,7 @@
       <c r="Q49" s="13"/>
       <c r="R49" s="11"/>
       <c r="S49" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="T49" s="11"/>
       <c r="U49" s="11"/>
@@ -6191,7 +6188,7 @@
       <c r="X49" s="13"/>
       <c r="Y49" s="11"/>
       <c r="Z49" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AA49" s="11"/>
       <c r="AB49" s="11"/>
@@ -6204,27 +6201,27 @@
       <c r="AI49" s="11"/>
       <c r="AJ49" s="11"/>
       <c r="AK49" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AL49" s="11"/>
       <c r="AM49" s="11"/>
     </row>
     <row r="50" spans="1:39" s="15" customFormat="1">
       <c r="A50" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B50" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D50" s="17"/>
       <c r="E50" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G50" s="11" t="s">
         <v>88</v>
@@ -6272,20 +6269,20 @@
     </row>
     <row r="51" spans="1:39" s="15" customFormat="1">
       <c r="A51" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B51" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D51" s="17"/>
       <c r="E51" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F51" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G51" s="11" t="s">
         <v>88</v>
@@ -6333,20 +6330,20 @@
     </row>
     <row r="52" spans="1:39" s="15" customFormat="1">
       <c r="A52" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B52" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D52" s="17"/>
       <c r="E52" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G52" s="11" t="s">
         <v>88</v>
@@ -6394,20 +6391,20 @@
     </row>
     <row r="53" spans="1:39" s="15" customFormat="1">
       <c r="A53" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B53" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D53" s="17"/>
       <c r="E53" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F53" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G53" s="11" t="s">
         <v>88</v>
@@ -6461,30 +6458,30 @@
         <v>41</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>89</v>
       </c>
       <c r="H54" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I54" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="J54" s="9"/>
       <c r="K54" s="1"/>
       <c r="L54" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
@@ -6518,20 +6515,20 @@
     </row>
     <row r="55" spans="1:39">
       <c r="A55" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D55" s="17"/>
       <c r="E55" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>2</v>
@@ -6540,13 +6537,13 @@
       <c r="I55" s="1"/>
       <c r="J55" s="9"/>
       <c r="K55" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="M55" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="L55" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="M55" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="N55" s="1" t="s">
         <v>99</v>
@@ -6555,13 +6552,13 @@
       <c r="P55" s="1"/>
       <c r="Q55" s="9"/>
       <c r="R55" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="S55" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="T55" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="U55" s="1" t="s">
         <v>91</v>
@@ -6587,20 +6584,20 @@
     </row>
     <row r="56" spans="1:39" ht="45">
       <c r="A56" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D56" s="17"/>
       <c r="E56" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>2</v>
@@ -6612,7 +6609,7 @@
         <v>3</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
@@ -6644,20 +6641,20 @@
     </row>
     <row r="57" spans="1:39">
       <c r="A57" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D57" s="17"/>
       <c r="E57" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>2</v>
@@ -6669,7 +6666,7 @@
         <v>3</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
@@ -6707,14 +6704,14 @@
         <v>41</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D58" s="17"/>
       <c r="E58" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>2</v>
@@ -6726,7 +6723,7 @@
         <v>97</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M58" s="1" t="s">
         <v>68</v>
@@ -6741,7 +6738,7 @@
         <v>107</v>
       </c>
       <c r="S58" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="T58" s="1" t="s">
         <v>68</v>
@@ -6770,7 +6767,7 @@
     </row>
     <row r="59" spans="1:39">
       <c r="A59" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>41</v>
@@ -6780,10 +6777,10 @@
       </c>
       <c r="D59" s="17"/>
       <c r="E59" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>2</v>
@@ -6795,7 +6792,7 @@
         <v>3</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M59" s="1"/>
       <c r="N59" s="1"/>
@@ -6827,20 +6824,20 @@
     </row>
     <row r="60" spans="1:39" ht="30">
       <c r="A60" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C60" s="19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D60" s="17"/>
       <c r="E60" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>2</v>
@@ -6852,7 +6849,7 @@
         <v>3</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M60" s="1"/>
       <c r="N60" s="1"/>
@@ -6884,20 +6881,20 @@
     </row>
     <row r="61" spans="1:39" ht="45">
       <c r="A61" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C61" s="19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D61" s="17"/>
       <c r="E61" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>2</v>
@@ -6909,7 +6906,7 @@
         <v>3</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="M61" s="1"/>
       <c r="N61" s="1"/>
@@ -6941,20 +6938,20 @@
     </row>
     <row r="62" spans="1:39" ht="45">
       <c r="A62" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C62" s="19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D62" s="17"/>
       <c r="E62" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>2</v>
@@ -6966,7 +6963,7 @@
         <v>3</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="M62" s="1"/>
       <c r="N62" s="1"/>
@@ -6998,20 +6995,20 @@
     </row>
     <row r="63" spans="1:39">
       <c r="A63" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C63" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D63" s="17"/>
       <c r="E63" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>2</v>
@@ -7023,7 +7020,7 @@
         <v>3</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="M63" s="1"/>
       <c r="N63" s="1"/>
@@ -7061,30 +7058,30 @@
         <v>41</v>
       </c>
       <c r="C64" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D64" s="17" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>89</v>
       </c>
       <c r="H64" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I64" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="I64" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="J64" s="9"/>
       <c r="K64" s="1"/>
       <c r="L64" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M64" s="1"/>
       <c r="N64" s="1"/>
@@ -7111,27 +7108,27 @@
       <c r="AI64" s="1"/>
       <c r="AJ64" s="1"/>
       <c r="AK64" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AL64" s="1"/>
       <c r="AM64" s="1"/>
     </row>
     <row r="65" spans="1:39">
       <c r="A65" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C65" s="19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D65" s="17"/>
       <c r="E65" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>2</v>
@@ -7140,10 +7137,10 @@
       <c r="I65" s="1"/>
       <c r="J65" s="9"/>
       <c r="K65" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M65" s="1"/>
       <c r="N65" s="1"/>
@@ -7151,10 +7148,10 @@
       <c r="P65" s="1"/>
       <c r="Q65" s="9"/>
       <c r="R65" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="S65" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T65" s="1"/>
       <c r="U65" s="1"/>
@@ -7179,20 +7176,20 @@
     </row>
     <row r="66" spans="1:39" ht="30">
       <c r="A66" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C66" s="19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D66" s="17"/>
       <c r="E66" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>2</v>
@@ -7204,7 +7201,7 @@
         <v>3</v>
       </c>
       <c r="L66" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M66" s="1"/>
       <c r="N66" s="1"/>
@@ -7236,34 +7233,34 @@
     </row>
     <row r="67" spans="1:39">
       <c r="A67" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C67" s="19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D67" s="17"/>
       <c r="E67" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>89</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J67" s="9"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M67" s="1"/>
       <c r="N67" s="1"/>
@@ -7290,27 +7287,27 @@
       <c r="AI67" s="1"/>
       <c r="AJ67" s="1"/>
       <c r="AK67" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AL67" s="1"/>
       <c r="AM67" s="1"/>
     </row>
     <row r="68" spans="1:39">
       <c r="A68" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C68" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D68" s="17"/>
       <c r="E68" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>2</v>
@@ -7322,7 +7319,7 @@
         <v>3</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M68" s="1"/>
       <c r="N68" s="1"/>
@@ -7354,20 +7351,20 @@
     </row>
     <row r="69" spans="1:39" ht="45">
       <c r="A69" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C69" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D69" s="17"/>
       <c r="E69" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>2</v>
@@ -7379,7 +7376,7 @@
         <v>3</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M69" s="1"/>
       <c r="N69" s="1"/>
@@ -7411,7 +7408,7 @@
     </row>
     <row r="70" spans="1:39">
       <c r="A70" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>41</v>
@@ -7423,10 +7420,10 @@
         <v>87</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>2</v>
@@ -7476,28 +7473,28 @@
         <v>41</v>
       </c>
       <c r="C71" s="19" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D71" s="17"/>
       <c r="E71" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G71" s="11" t="s">
         <v>89</v>
       </c>
       <c r="H71" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="I71" s="11" t="s">
         <v>244</v>
-      </c>
-      <c r="I71" s="11" t="s">
-        <v>245</v>
       </c>
       <c r="J71" s="13"/>
       <c r="K71" s="11"/>
       <c r="L71" s="11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="M71" s="11"/>
       <c r="N71" s="11"/>
@@ -7524,27 +7521,27 @@
       <c r="AI71" s="11"/>
       <c r="AJ71" s="11"/>
       <c r="AK71" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AL71" s="11"/>
       <c r="AM71" s="11"/>
     </row>
     <row r="72" spans="1:39" s="15" customFormat="1" ht="45">
       <c r="A72" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B72" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C72" s="19" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D72" s="17"/>
       <c r="E72" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F72" s="11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G72" s="11" t="s">
         <v>2</v>
@@ -7556,7 +7553,7 @@
         <v>3</v>
       </c>
       <c r="L72" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M72" s="11"/>
       <c r="N72" s="11"/>
@@ -7588,20 +7585,20 @@
     </row>
     <row r="73" spans="1:39" s="15" customFormat="1">
       <c r="A73" s="11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B73" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C73" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D73" s="17"/>
       <c r="E73" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F73" s="11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G73" s="11" t="s">
         <v>89</v>
@@ -7615,7 +7612,7 @@
       <c r="J73" s="13"/>
       <c r="K73" s="11"/>
       <c r="L73" s="11" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="M73" s="11"/>
       <c r="N73" s="11"/>
@@ -7628,7 +7625,7 @@
       <c r="Q73" s="13"/>
       <c r="R73" s="11"/>
       <c r="S73" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="T73" s="11"/>
       <c r="U73" s="11"/>
@@ -7641,7 +7638,7 @@
       <c r="X73" s="13"/>
       <c r="Y73" s="11"/>
       <c r="Z73" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AA73" s="11"/>
       <c r="AB73" s="11"/>
@@ -7654,27 +7651,27 @@
       <c r="AI73" s="11"/>
       <c r="AJ73" s="11"/>
       <c r="AK73" s="11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AL73" s="11"/>
       <c r="AM73" s="11"/>
     </row>
     <row r="74" spans="1:39" s="15" customFormat="1">
       <c r="A74" s="11" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B74" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C74" s="19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D74" s="17"/>
       <c r="E74" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="F74" s="11" t="s">
         <v>295</v>
-      </c>
-      <c r="F74" s="11" t="s">
-        <v>296</v>
       </c>
       <c r="G74" s="11" t="s">
         <v>2</v>
@@ -7686,7 +7683,7 @@
         <v>3</v>
       </c>
       <c r="L74" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M74" s="11"/>
       <c r="N74" s="11"/>
@@ -7718,20 +7715,20 @@
     </row>
     <row r="75" spans="1:39" s="15" customFormat="1">
       <c r="A75" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B75" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C75" s="19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D75" s="17"/>
       <c r="E75" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="F75" s="11" t="s">
         <v>295</v>
-      </c>
-      <c r="F75" s="11" t="s">
-        <v>296</v>
       </c>
       <c r="G75" s="11" t="s">
         <v>2</v>
@@ -7743,7 +7740,7 @@
         <v>3</v>
       </c>
       <c r="L75" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M75" s="11"/>
       <c r="N75" s="11"/>
@@ -7775,20 +7772,20 @@
     </row>
     <row r="76" spans="1:39" s="15" customFormat="1">
       <c r="A76" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B76" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C76" s="19" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D76" s="17"/>
       <c r="E76" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="F76" s="11" t="s">
         <v>295</v>
-      </c>
-      <c r="F76" s="11" t="s">
-        <v>296</v>
       </c>
       <c r="G76" s="11" t="s">
         <v>2</v>
@@ -7800,7 +7797,7 @@
         <v>3</v>
       </c>
       <c r="L76" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M76" s="11"/>
       <c r="N76" s="11"/>
@@ -7832,20 +7829,20 @@
     </row>
     <row r="77" spans="1:39" s="15" customFormat="1">
       <c r="A77" s="11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B77" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C77" s="19" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D77" s="17"/>
       <c r="E77" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="F77" s="11" t="s">
         <v>295</v>
-      </c>
-      <c r="F77" s="11" t="s">
-        <v>296</v>
       </c>
       <c r="G77" s="11" t="s">
         <v>2</v>
@@ -7854,10 +7851,10 @@
       <c r="I77" s="11"/>
       <c r="J77" s="13"/>
       <c r="K77" s="11" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="L77" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M77" s="11"/>
       <c r="N77" s="11"/>
@@ -7889,26 +7886,26 @@
     </row>
     <row r="78" spans="1:39" s="15" customFormat="1">
       <c r="A78" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B78" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C78" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D78" s="17"/>
       <c r="E78" s="11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F78" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G78" s="11" t="s">
         <v>89</v>
       </c>
       <c r="H78" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I78" s="11" t="s">
         <v>91</v>
@@ -7916,7 +7913,7 @@
       <c r="J78" s="13"/>
       <c r="K78" s="11"/>
       <c r="L78" s="11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M78" s="11"/>
       <c r="N78" s="11"/>
@@ -7943,27 +7940,27 @@
       <c r="AI78" s="11"/>
       <c r="AJ78" s="11"/>
       <c r="AK78" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AL78" s="11"/>
       <c r="AM78" s="11"/>
     </row>
     <row r="79" spans="1:39" s="15" customFormat="1" ht="45">
       <c r="A79" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B79" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C79" s="19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D79" s="17"/>
       <c r="E79" s="11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F79" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G79" s="11" t="s">
         <v>2</v>
@@ -7975,7 +7972,7 @@
         <v>3</v>
       </c>
       <c r="L79" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M79" s="11"/>
       <c r="N79" s="11"/>
@@ -8007,20 +8004,20 @@
     </row>
     <row r="80" spans="1:39" s="15" customFormat="1">
       <c r="A80" s="11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B80" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C80" s="19" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D80" s="17"/>
       <c r="E80" s="11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F80" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G80" s="11" t="s">
         <v>2</v>
@@ -8032,7 +8029,7 @@
         <v>3</v>
       </c>
       <c r="L80" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M80" s="11"/>
       <c r="N80" s="11"/>
@@ -8064,20 +8061,20 @@
     </row>
     <row r="81" spans="1:39" s="15" customFormat="1">
       <c r="A81" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B81" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C81" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D81" s="17"/>
       <c r="E81" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F81" s="11" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G81" s="11" t="s">
         <v>2</v>
@@ -8089,7 +8086,7 @@
         <v>3</v>
       </c>
       <c r="L81" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M81" s="11"/>
       <c r="N81" s="11"/>
@@ -8121,20 +8118,20 @@
     </row>
     <row r="82" spans="1:39">
       <c r="A82" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C82" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D82" s="17"/>
       <c r="E82" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>88</v>
@@ -8146,7 +8143,7 @@
       </c>
       <c r="K82" s="1"/>
       <c r="L82" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M82" s="1"/>
       <c r="N82" s="1"/>
@@ -8157,7 +8154,7 @@
       </c>
       <c r="R82" s="1"/>
       <c r="S82" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="T82" s="1"/>
       <c r="U82" s="1"/>
@@ -8182,20 +8179,20 @@
     </row>
     <row r="83" spans="1:39">
       <c r="A83" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C83" s="19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D83" s="17"/>
       <c r="E83" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>88</v>
@@ -8207,7 +8204,7 @@
       </c>
       <c r="K83" s="1"/>
       <c r="L83" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M83" s="1"/>
       <c r="N83" s="1"/>
@@ -8218,7 +8215,7 @@
       </c>
       <c r="R83" s="1"/>
       <c r="S83" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="T83" s="1"/>
       <c r="U83" s="1"/>
@@ -8243,22 +8240,22 @@
     </row>
     <row r="84" spans="1:39">
       <c r="A84" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C84" s="19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D84" s="17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G84" s="1" t="s">
         <v>2</v>
@@ -8270,7 +8267,7 @@
         <v>3</v>
       </c>
       <c r="L84" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M84" s="1"/>
       <c r="N84" s="1"/>
@@ -8302,22 +8299,22 @@
     </row>
     <row r="85" spans="1:39">
       <c r="A85" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C85" s="19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D85" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G85" s="1" t="s">
         <v>88</v>
@@ -8329,13 +8326,13 @@
       </c>
       <c r="K85" s="1"/>
       <c r="L85" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="M85" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N85" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O85" s="1"/>
       <c r="P85" s="1"/>
@@ -8344,7 +8341,7 @@
       </c>
       <c r="R85" s="1"/>
       <c r="S85" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T85" s="1"/>
       <c r="U85" s="1"/>
@@ -8369,20 +8366,20 @@
     </row>
     <row r="86" spans="1:39">
       <c r="A86" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C86" s="19" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D86" s="17"/>
       <c r="E86" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G86" s="1" t="s">
         <v>88</v>
@@ -8394,7 +8391,7 @@
       </c>
       <c r="K86" s="1"/>
       <c r="L86" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M86" s="1"/>
       <c r="N86" s="1"/>
@@ -8405,7 +8402,7 @@
       </c>
       <c r="R86" s="1"/>
       <c r="S86" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="T86" s="1"/>
       <c r="U86" s="1"/>
@@ -8416,7 +8413,7 @@
       </c>
       <c r="Y86" s="1"/>
       <c r="Z86" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AA86" s="1"/>
       <c r="AB86" s="1"/>
@@ -8434,20 +8431,20 @@
     </row>
     <row r="87" spans="1:39">
       <c r="A87" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C87" s="19" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D87" s="17"/>
       <c r="E87" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>2</v>
@@ -8459,7 +8456,7 @@
         <v>3</v>
       </c>
       <c r="L87" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M87" s="1"/>
       <c r="N87" s="1"/>
@@ -8491,20 +8488,20 @@
     </row>
     <row r="88" spans="1:39">
       <c r="A88" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C88" s="19" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D88" s="17"/>
       <c r="E88" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G88" s="1" t="s">
         <v>88</v>
@@ -8516,13 +8513,13 @@
       </c>
       <c r="K88" s="1"/>
       <c r="L88" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M88" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="N88" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="N88" s="1" t="s">
-        <v>231</v>
       </c>
       <c r="O88" s="1"/>
       <c r="P88" s="1"/>
@@ -8531,7 +8528,7 @@
       </c>
       <c r="R88" s="1"/>
       <c r="S88" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T88" s="1"/>
       <c r="U88" s="1"/>
@@ -8556,20 +8553,20 @@
     </row>
     <row r="89" spans="1:39">
       <c r="A89" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C89" s="19" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D89" s="17"/>
       <c r="E89" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G89" s="1" t="s">
         <v>2</v>
@@ -8581,7 +8578,7 @@
         <v>3</v>
       </c>
       <c r="L89" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M89" s="1"/>
       <c r="N89" s="1"/>
@@ -8613,20 +8610,20 @@
     </row>
     <row r="90" spans="1:39">
       <c r="A90" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C90" s="19" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D90" s="17"/>
       <c r="E90" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>2</v>
@@ -8670,20 +8667,20 @@
     </row>
     <row r="91" spans="1:39">
       <c r="A91" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C91" s="19" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D91" s="17"/>
       <c r="E91" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>2</v>
@@ -8733,43 +8730,43 @@
         <v>41</v>
       </c>
       <c r="C92" s="19" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D92" s="17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G92" s="1" t="s">
         <v>89</v>
       </c>
       <c r="H92" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="I92" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="I92" s="1" t="s">
-        <v>231</v>
       </c>
       <c r="J92" s="9"/>
       <c r="K92" s="1"/>
       <c r="L92" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M92" s="1"/>
       <c r="N92" s="1"/>
       <c r="O92" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="P92" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Q92" s="9"/>
       <c r="R92" s="1"/>
       <c r="S92" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="T92" s="1"/>
       <c r="U92" s="1"/>
@@ -8794,20 +8791,20 @@
     </row>
     <row r="93" spans="1:39">
       <c r="A93" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C93" s="19" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D93" s="17"/>
       <c r="E93" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>88</v>
@@ -8819,7 +8816,7 @@
       </c>
       <c r="K93" s="1"/>
       <c r="L93" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M93" s="1"/>
       <c r="N93" s="1"/>
@@ -8830,7 +8827,7 @@
       </c>
       <c r="R93" s="1"/>
       <c r="S93" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="T93" s="1"/>
       <c r="U93" s="1"/>
@@ -8855,20 +8852,20 @@
     </row>
     <row r="94" spans="1:39">
       <c r="A94" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C94" s="19" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D94" s="17"/>
       <c r="E94" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>88</v>
@@ -8880,7 +8877,7 @@
       </c>
       <c r="K94" s="1"/>
       <c r="L94" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M94" s="1"/>
       <c r="N94" s="1"/>
@@ -8891,7 +8888,7 @@
       </c>
       <c r="R94" s="1"/>
       <c r="S94" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="T94" s="1"/>
       <c r="U94" s="1"/>
@@ -8916,7 +8913,7 @@
     </row>
     <row r="95" spans="1:39">
       <c r="A95" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>41</v>
@@ -8926,10 +8923,10 @@
       </c>
       <c r="D95" s="17"/>
       <c r="E95" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G95" s="1" t="s">
         <v>2</v>
@@ -8973,20 +8970,20 @@
     </row>
     <row r="96" spans="1:39">
       <c r="A96" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C96" s="19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D96" s="17"/>
       <c r="E96" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>2</v>
@@ -9030,22 +9027,22 @@
     </row>
     <row r="97" spans="1:39">
       <c r="A97" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C97" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D97" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G97" s="1" t="s">
         <v>2</v>
@@ -9095,14 +9092,14 @@
         <v>78</v>
       </c>
       <c r="C98" s="19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D98" s="17"/>
       <c r="E98" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>2</v>
@@ -9148,14 +9145,14 @@
         <v>78</v>
       </c>
       <c r="C99" s="19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D99" s="17"/>
       <c r="E99" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G99" s="1" t="s">
         <v>2</v>
@@ -9201,14 +9198,14 @@
         <v>78</v>
       </c>
       <c r="C100" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D100" s="17"/>
       <c r="E100" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G100" s="1" t="s">
         <v>2</v>
@@ -9248,20 +9245,20 @@
     </row>
     <row r="101" spans="1:39">
       <c r="A101" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C101" s="19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D101" s="17"/>
       <c r="E101" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G101" s="1" t="s">
         <v>2</v>
@@ -9311,14 +9308,14 @@
         <v>78</v>
       </c>
       <c r="C102" s="19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D102" s="17"/>
       <c r="E102" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G102" s="1" t="s">
         <v>2</v>
@@ -9358,20 +9355,20 @@
     </row>
     <row r="103" spans="1:39">
       <c r="A103" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B103" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C103" s="19" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D103" s="17"/>
       <c r="E103" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G103" s="1" t="s">
         <v>2</v>
@@ -9420,14 +9417,14 @@
         <v>78</v>
       </c>
       <c r="C104" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D104" s="17"/>
       <c r="E104" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G104" s="1" t="s">
         <v>2</v>
@@ -9467,20 +9464,20 @@
     </row>
     <row r="105" spans="1:39" ht="45">
       <c r="A105" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C105" s="19" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D105" s="17"/>
       <c r="E105" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G105" s="1" t="s">
         <v>2</v>
@@ -9529,14 +9526,14 @@
         <v>78</v>
       </c>
       <c r="C106" s="19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D106" s="17"/>
       <c r="E106" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G106" s="1" t="s">
         <v>2</v>

</xml_diff>